<commit_message>
Updated power system BOM in GROUP9_BOM
</commit_message>
<xml_diff>
--- a/Other/GROUP9_BOM.xlsx
+++ b/Other/GROUP9_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidyoung/Desktop/UCT/3rd Year 1st Semester (2022)/EEE3088F/EEE3088F-Team-9/Other/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Desktop\EEE Stuff\EEE3088F\Project\EEE3088F-Team-9\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C7198E-3E13-E64A-9136-DF3E9F595F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CDAB79-E65D-486B-ABD9-F9ED272BCAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15060" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -637,21 +637,21 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -685,11 +685,11 @@
         <v>0.01</v>
       </c>
       <c r="F2">
-        <f>(D2*E2)</f>
+        <f t="shared" ref="F2:F8" si="0">(D2*E2)</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>68</v>
@@ -704,11 +704,11 @@
         <v>0.01</v>
       </c>
       <c r="F3">
-        <f>(D3*E3)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>57</v>
@@ -723,11 +723,11 @@
         <v>0.01</v>
       </c>
       <c r="F4">
-        <f>(D4*E4)</f>
+        <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>59</v>
@@ -742,11 +742,11 @@
         <v>0.01</v>
       </c>
       <c r="F5">
-        <f>(D5*E5)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>60</v>
@@ -761,11 +761,11 @@
         <v>0.01</v>
       </c>
       <c r="F6">
-        <f>(D6*E6)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>63</v>
@@ -780,11 +780,11 @@
         <v>0.01</v>
       </c>
       <c r="F7">
-        <f>(D7*E7)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>51</v>
@@ -799,11 +799,11 @@
         <v>0.01</v>
       </c>
       <c r="F8">
-        <f>(D8*E8)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>49</v>
       </c>
@@ -817,11 +817,11 @@
         <v>0.01</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F20" si="0">(D9*E9)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F9:F20" si="1">(D9*E9)</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>52</v>
       </c>
@@ -835,11 +835,11 @@
         <v>0.01</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>54</v>
       </c>
@@ -853,11 +853,11 @@
         <v>0.01</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F12" si="1">(D11*E11)</f>
+        <f t="shared" ref="F11:F12" si="2">(D11*E11)</f>
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -871,11 +871,11 @@
         <v>0.01</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>56</v>
       </c>
@@ -889,11 +889,11 @@
         <v>0.01</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13" si="2">(D13*E13)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F13" si="3">(D13*E13)</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -907,11 +907,11 @@
         <v>0.04</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -925,11 +925,11 @@
         <v>0.25</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -943,11 +943,11 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -961,14 +961,14 @@
         <v>0.22</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.22</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -982,14 +982,14 @@
         <v>0.3</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -997,17 +997,17 @@
         <v>16</v>
       </c>
       <c r="D19" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>0.17</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -1021,14 +1021,14 @@
         <v>1.6</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1037,13 +1037,13 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F2:F20)</f>
-        <v>3.09</v>
+        <v>2.92</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1060,11 +1060,11 @@
         <v>1.8800000000000001E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:F29" si="3">(D23*E23)</f>
+        <f t="shared" ref="F23:F29" si="4">(D23*E23)</f>
         <v>5.6400000000000006E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>49</v>
@@ -1079,11 +1079,11 @@
         <v>0.01</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -1097,11 +1097,11 @@
         <v>0.01</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>27</v>
       </c>
@@ -1115,11 +1115,11 @@
         <v>0.01</v>
       </c>
       <c r="F26">
-        <f t="shared" si="3"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>34</v>
       </c>
@@ -1133,11 +1133,11 @@
         <v>1.5556000000000001</v>
       </c>
       <c r="F27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5556000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>33</v>
       </c>
@@ -1151,11 +1151,11 @@
         <v>3.7227000000000001</v>
       </c>
       <c r="F28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7227000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>70</v>
       </c>
@@ -1169,14 +1169,14 @@
         <v>4.9599999999999998E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.9599999999999998E-2</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>57</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>36</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>19</v>
       </c>
@@ -1227,10 +1227,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>27</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>40</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>44</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
@@ -1326,10 +1326,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="F40" s="7">
         <f>SUM(F32+F38+F21)</f>
-        <v>12.281499999999999</v>
+        <v>12.111499999999999</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Added MCP6002 OpAmp files
</commit_message>
<xml_diff>
--- a/Other/GROUP9_BOM.xlsx
+++ b/Other/GROUP9_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Desktop\EEE Stuff\EEE3088F\Project\EEE3088F-Team-9\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidyoung/Desktop/UCT/3rd Year 1st Semester (2022)/EEE3088F/EEE3088F-Team-9/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CDAB79-E65D-486B-ABD9-F9ED272BCAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8920C0-3F90-4E40-8551-9D210F67D5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40620" yWindow="-220" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>Component Name</t>
   </si>
@@ -61,12 +61,6 @@
     <t>C16581</t>
   </si>
   <si>
-    <t>C7950</t>
-  </si>
-  <si>
-    <t>LM358 Op-amp</t>
-  </si>
-  <si>
     <t>Inductor</t>
   </si>
   <si>
@@ -251,6 +245,18 @@
   </si>
   <si>
     <t>C84256</t>
+  </si>
+  <si>
+    <t>C7377</t>
+  </si>
+  <si>
+    <t>MCP6002 Op-amp</t>
+  </si>
+  <si>
+    <t>10kΩ Resistor</t>
+  </si>
+  <si>
+    <t>C25804</t>
   </si>
 </sst>
 </file>
@@ -634,24 +640,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +665,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -668,15 +674,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -689,13 +695,13 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -708,13 +714,13 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -727,13 +733,13 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -746,13 +752,13 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -765,13 +771,13 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -784,13 +790,13 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -803,12 +809,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -821,12 +827,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -839,12 +845,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -857,12 +863,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -875,12 +881,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -893,7 +899,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -911,7 +917,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -929,30 +935,30 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>0.14000000000000001</v>
+        <v>0.40350000000000003</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.40350000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -965,15 +971,15 @@
         <v>0.22</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -986,15 +992,15 @@
         <v>0.3</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -1007,12 +1013,12 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -1025,33 +1031,33 @@
         <v>1.6</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F21" s="7">
         <f>SUM(F2:F20)</f>
-        <v>2.92</v>
+        <v>3.1835</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D23" s="4">
         <v>3</v>
@@ -1064,67 +1070,67 @@
         <v>5.6400000000000006E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24">
-        <v>0.01</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5.9200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>0.01</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -1137,12 +1143,12 @@
         <v>1.5556000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
         <v>33</v>
-      </c>
-      <c r="C28" t="s">
-        <v>35</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
@@ -1155,12 +1161,12 @@
         <v>3.7227000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
@@ -1173,175 +1179,193 @@
         <v>4.9599999999999998E-2</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>0.01</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F30">
         <f>(D30*E30)</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>0.01</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="F31">
         <f>(D31*E31)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="7">
-        <f>SUM(F23:F31)</f>
-        <v>5.4642999999999997</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>0.01</v>
-      </c>
-      <c r="F34">
-        <f>(D34*E34)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F32">
+        <f>(D32*E32)</f>
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="7">
+        <f>SUM(F23:F32)</f>
+        <v>5.4586000000000006</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="F35">
         <f>(D35*E35)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>2.6886000000000001</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="F36">
         <f>(D36*E36)</f>
-        <v>2.6886000000000001</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>1.0185999999999999</v>
+        <v>2.6886000000000001</v>
       </c>
       <c r="F37">
         <f>(D37*E37)</f>
+        <v>2.6886000000000001</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38">
         <v>1.0185999999999999</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="7">
-        <f>SUM(F34:F37)</f>
-        <v>3.7271999999999998</v>
+      <c r="F38">
+        <f>(D38*E38)</f>
+        <v>1.0185999999999999</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="7">
-        <f>SUM(F32+F38+F21)</f>
-        <v>12.111499999999999</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>46</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="7">
+        <f>SUM(F35:F38)</f>
+        <v>3.7137000000000002</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="7">
+        <f>SUM(F33+F39+F21)</f>
+        <v>12.3558</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Gerbers and updated BOM
</commit_message>
<xml_diff>
--- a/Other/GROUP9_BOM.xlsx
+++ b/Other/GROUP9_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidyoung/Desktop/UCT/3rd Year 1st Semester (2022)/EEE3088F/EEE3088F-Team-9/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8920C0-3F90-4E40-8551-9D210F67D5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44523310-C4CF-B445-8979-0AC96D1674A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40620" yWindow="-220" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-220" windowWidth="33000" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Component Name</t>
   </si>
@@ -79,9 +79,6 @@
     <t>P-channel MOSFET</t>
   </si>
   <si>
-    <t>C15127</t>
-  </si>
-  <si>
     <t>Voltage regulator</t>
   </si>
   <si>
@@ -142,15 +139,9 @@
     <t>4.7kΩ Resistor</t>
   </si>
   <si>
-    <t>C17673</t>
-  </si>
-  <si>
     <t>plus $3 Ext</t>
   </si>
   <si>
-    <t>100nF Capacitor</t>
-  </si>
-  <si>
     <t>Barometer (LPS22HBTR)</t>
   </si>
   <si>
@@ -208,24 +199,15 @@
     <t>C22765</t>
   </si>
   <si>
-    <t>1.8kΩ  Resistor</t>
-  </si>
-  <si>
     <t>100kΩ  Resistor</t>
   </si>
   <si>
-    <t>C4177</t>
-  </si>
-  <si>
     <t>C17900</t>
   </si>
   <si>
     <t>33kΩ  Resistor</t>
   </si>
   <si>
-    <t>C17633</t>
-  </si>
-  <si>
     <t>C12891</t>
   </si>
   <si>
@@ -235,12 +217,6 @@
     <t>C47339</t>
   </si>
   <si>
-    <t>120Ω Resistor</t>
-  </si>
-  <si>
-    <t>C22787</t>
-  </si>
-  <si>
     <t>USB Connector (MicroXNJ)</t>
   </si>
   <si>
@@ -257,6 +233,21 @@
   </si>
   <si>
     <t>C25804</t>
+  </si>
+  <si>
+    <t>0.1uF Capacitor</t>
+  </si>
+  <si>
+    <t>C4216</t>
+  </si>
+  <si>
+    <t>C8492</t>
+  </si>
+  <si>
+    <t>C23162</t>
+  </si>
+  <si>
+    <t>5 Board Total</t>
   </si>
 </sst>
 </file>
@@ -640,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -657,7 +648,7 @@
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -674,698 +665,675 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F8" si="0">(D2*E2)</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F2:F6" si="0">(D2*E2)</f>
+        <v>1.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.01</v>
+        <v>3.8E-3</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.01</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.01</v>
+        <v>1.3599999999999999E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+        <v>1.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.01</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+        <f t="shared" ref="F7:F18" si="1">(D7*E7)</f>
+        <v>2.9600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.1227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0.01</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>0.01</v>
+        <v>7.3499999999999996E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F20" si="1">(D9*E9)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F9:F10" si="2">(D9*E9)</f>
+        <v>0.22049999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>50</v>
       </c>
       <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>0.01</v>
-      </c>
-      <c r="F10">
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2E-3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11" si="3">(D11*E11)</f>
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="1"/>
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" t="s">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>63</v>
       </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>0.01</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ref="F11:F12" si="2">(D11*E11)</f>
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0.01</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0.01</v>
-      </c>
-      <c r="F13">
-        <f t="shared" ref="F13" si="3">(D13*E13)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
+      <c r="C14" t="s">
+        <v>62</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0.04</v>
+        <v>0.40350000000000003</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.40350000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>0.25</v>
+        <v>0.2225</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.2225</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>0.40350000000000003</v>
+        <v>0.29370000000000002</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0.40350000000000003</v>
+        <v>0.29370000000000002</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0.22</v>
+        <v>2.7300000000000001E-2</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0.22</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>10</v>
+        <v>2.7300000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>0.3</v>
+        <v>1.4948999999999999</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>1.4948999999999999</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>0.17</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1.6</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>1.6</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>10</v>
+      <c r="E19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="7">
+        <f>SUM(F2:F18)</f>
+        <v>3.1570999999999998</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="7">
-        <f>SUM(F2:F20)</f>
-        <v>3.1835</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>19</v>
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F27" si="4">(D21*E21)</f>
+        <v>5.28E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>5.9200000000000003E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>1E-3</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="4">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>1.8800000000000001E-2</v>
-      </c>
-      <c r="F23">
-        <f t="shared" ref="F23:F29" si="4">(D23*E23)</f>
-        <v>5.6400000000000006E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>2.9600000000000001E-2</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>5.9200000000000003E-2</v>
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
       </c>
-      <c r="D25">
-        <v>2</v>
+      <c r="D25" s="4">
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1E-3</v>
+        <v>1.4287000000000001</v>
       </c>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>2E-3</v>
+        <v>1.4287000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26">
+        <v>32</v>
+      </c>
+      <c r="D26" s="4">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>5.4999999999999997E-3</v>
+        <v>3.5501999999999998</v>
       </c>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>5.4999999999999997E-3</v>
+        <v>3.5501999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>1.5556000000000001</v>
+        <v>4.7E-2</v>
       </c>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>1.5556000000000001</v>
+        <v>4.7E-2</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
       </c>
       <c r="E28">
-        <v>3.7227000000000001</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F28">
-        <f t="shared" si="4"/>
-        <v>3.7227000000000001</v>
+        <f>(D28*E28)</f>
+        <v>2.5999999999999999E-3</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>4.9599999999999998E-2</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F29">
-        <f t="shared" si="4"/>
-        <v>4.9599999999999998E-2</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>10</v>
+        <f>(D29*E29)</f>
+        <v>1.1999999999999999E-3</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30">
+        <v>65</v>
+      </c>
+      <c r="D30" s="4">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>1.2999999999999999E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F30">
         <f>(D30*E30)</f>
-        <v>2.5999999999999999E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="7">
+        <f>SUM(F21:F30)</f>
+        <v>5.1515999999999993</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1E-3</v>
+      </c>
+      <c r="F33">
+        <f>(D33*E33)</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="F34">
+        <f>(D34*E34)</f>
+        <v>5.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="4">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="F31">
-        <f>(D31*E31)</f>
-        <v>2.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="4">
-        <v>2</v>
-      </c>
-      <c r="E32">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F32">
-        <f>(D32*E32)</f>
-        <v>2.3999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="7">
-        <f>SUM(F23:F32)</f>
-        <v>5.4586000000000006</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>1E-3</v>
+        <v>2.4323999999999999</v>
       </c>
       <c r="F35">
         <f>(D35*E35)</f>
-        <v>1E-3</v>
+        <v>2.4323999999999999</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36">
+        <v>36</v>
+      </c>
+      <c r="D36" s="4">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>5.4999999999999997E-3</v>
+        <v>0.97230000000000005</v>
       </c>
       <c r="F36">
         <f>(D36*E36)</f>
-        <v>5.4999999999999997E-3</v>
+        <v>0.97230000000000005</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>2.6886000000000001</v>
-      </c>
-      <c r="F37">
-        <f>(D37*E37)</f>
-        <v>2.6886000000000001</v>
+      <c r="B37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="7">
+        <f>SUM(F33:F36)</f>
+        <v>3.4112</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1.0185999999999999</v>
-      </c>
-      <c r="F38">
-        <f>(D38*E38)</f>
-        <v>1.0185999999999999</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="F39" s="7">
-        <f>SUM(F35:F38)</f>
-        <v>3.7137000000000002</v>
+        <f>SUM(F31+F37+F19)</f>
+        <v>11.719899999999999</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="7">
-        <f>SUM(F33+F39+F21)</f>
-        <v>12.3558</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>44</v>
+      <c r="B40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="7">
+        <f>SUM(F31+F37+F19)*5 + 6*3</f>
+        <v>76.599499999999992</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>